<commit_message>
v1.0.0 Done confirm pay
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42560739-8F36-4B33-9E9D-56408C1C2A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6821395-1737-4B3C-8C79-4AD051E421BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="213">
   <si>
     <t>id</t>
   </si>
@@ -522,6 +522,162 @@
   </si>
   <si>
     <t>รวมราคาสินค้า :</t>
+  </si>
+  <si>
+    <t>errName4to50</t>
+  </si>
+  <si>
+    <t>Name can only has 4 to 50 charactors.</t>
+  </si>
+  <si>
+    <t>ชื่อมีความยาวตั้งแต่ 4 ถึง 50 ตัวอักษร</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address.</t>
+  </si>
+  <si>
+    <t>errInvalidEmail</t>
+  </si>
+  <si>
+    <t>รูปแบบอีเมล์ไม่ถูกต้อง</t>
+  </si>
+  <si>
+    <t>errInvalidPhone</t>
+  </si>
+  <si>
+    <t>Please enter a valid phone number.</t>
+  </si>
+  <si>
+    <t>รูปแบบเบอร์ติดต่อไม่ถูกต้อง</t>
+  </si>
+  <si>
+    <t>errAddress20to400</t>
+  </si>
+  <si>
+    <t>Address must be between 20 and 400 characters</t>
+  </si>
+  <si>
+    <t>ที่อยู่สั้นหรือยาวเกินไป</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>remarkPH</t>
+  </si>
+  <si>
+    <t>Message to the seller</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>บันทึก</t>
+  </si>
+  <si>
+    <t>ข้อความถึงผู้ขาย</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>errTest</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>ผิดพลาด</t>
+  </si>
+  <si>
+    <t>ทดสอบผิดพลาด</t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+  <si>
+    <t>errInputMissing</t>
+  </si>
+  <si>
+    <t>ข้อมูลบางส่วนสูญหาย</t>
+  </si>
+  <si>
+    <t>Some information is missing</t>
+  </si>
+  <si>
+    <t>errMissing</t>
+  </si>
+  <si>
+    <t>errCartMissing</t>
+  </si>
+  <si>
+    <t>Some information is missing (input)</t>
+  </si>
+  <si>
+    <t>Some information is missing (cart)</t>
+  </si>
+  <si>
+    <t>ข้อมูลบางส่วนสูญหาย (input)</t>
+  </si>
+  <si>
+    <t>ข้อมูลบางส่วนสูญหาย (cart)</t>
+  </si>
+  <si>
+    <t>errInvalidProdectOptId</t>
+  </si>
+  <si>
+    <t>errTotalAmtMismatch</t>
+  </si>
+  <si>
+    <t>ผลรวมไม่สมเหตุผล</t>
+  </si>
+  <si>
+    <t>errGrandTotalMismatch</t>
+  </si>
+  <si>
+    <t>Total Amount Mismatch.</t>
+  </si>
+  <si>
+    <t>Grand Total Mismatch</t>
+  </si>
+  <si>
+    <t>ผลรวมสุดท้ายไม่สมเหตุผล</t>
+  </si>
+  <si>
+    <t>useQRPay</t>
+  </si>
+  <si>
+    <t>useManualPay</t>
+  </si>
+  <si>
+    <t>Switch to manual pay</t>
+  </si>
+  <si>
+    <t>Switch to QR pay</t>
+  </si>
+  <si>
+    <t>เปลี่ยนเป็นโอนด้วยเลขบัญชี</t>
+  </si>
+  <si>
+    <t>clickToUpload</t>
+  </si>
+  <si>
+    <t>Click to upload</t>
+  </si>
+  <si>
+    <t>คลิ๊กเพื่อส่งรูป</t>
+  </si>
+  <si>
+    <t>เปลี่ยนเป็นโอนด้วยคิวอาร์</t>
+  </si>
+  <si>
+    <t>totalForPay</t>
+  </si>
+  <si>
+    <t>Total Pay</t>
+  </si>
+  <si>
+    <t>ยอดรวม</t>
   </si>
 </sst>
 </file>
@@ -899,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2241,6 +2397,528 @@
         <v>158</v>
       </c>
     </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" t="s">
+        <v>162</v>
+      </c>
+      <c r="E47" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" t="s">
+        <v>162</v>
+      </c>
+      <c r="G47" t="s">
+        <v>162</v>
+      </c>
+      <c r="H47" t="s">
+        <v>162</v>
+      </c>
+      <c r="I47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" t="s">
+        <v>164</v>
+      </c>
+      <c r="H48" t="s">
+        <v>164</v>
+      </c>
+      <c r="I48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" t="s">
+        <v>168</v>
+      </c>
+      <c r="F49" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" t="s">
+        <v>168</v>
+      </c>
+      <c r="H49" t="s">
+        <v>168</v>
+      </c>
+      <c r="I49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" t="s">
+        <v>171</v>
+      </c>
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+      <c r="G50" t="s">
+        <v>171</v>
+      </c>
+      <c r="H50" t="s">
+        <v>171</v>
+      </c>
+      <c r="I50" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" t="s">
+        <v>177</v>
+      </c>
+      <c r="D51" t="s">
+        <v>176</v>
+      </c>
+      <c r="E51" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" t="s">
+        <v>176</v>
+      </c>
+      <c r="G51" t="s">
+        <v>176</v>
+      </c>
+      <c r="H51" t="s">
+        <v>176</v>
+      </c>
+      <c r="I51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" t="s">
+        <v>175</v>
+      </c>
+      <c r="F52" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" t="s">
+        <v>175</v>
+      </c>
+      <c r="H52" t="s">
+        <v>175</v>
+      </c>
+      <c r="I52" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" t="s">
+        <v>181</v>
+      </c>
+      <c r="E53" t="s">
+        <v>181</v>
+      </c>
+      <c r="F53" t="s">
+        <v>181</v>
+      </c>
+      <c r="G53" t="s">
+        <v>181</v>
+      </c>
+      <c r="H53" t="s">
+        <v>181</v>
+      </c>
+      <c r="I53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" t="s">
+        <v>183</v>
+      </c>
+      <c r="D54" t="s">
+        <v>184</v>
+      </c>
+      <c r="E54" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" t="s">
+        <v>184</v>
+      </c>
+      <c r="G54" t="s">
+        <v>184</v>
+      </c>
+      <c r="H54" t="s">
+        <v>184</v>
+      </c>
+      <c r="I54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" t="s">
+        <v>187</v>
+      </c>
+      <c r="E55" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" t="s">
+        <v>187</v>
+      </c>
+      <c r="G55" t="s">
+        <v>187</v>
+      </c>
+      <c r="H55" t="s">
+        <v>187</v>
+      </c>
+      <c r="I55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>185</v>
+      </c>
+      <c r="B56" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" t="s">
+        <v>192</v>
+      </c>
+      <c r="D56" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" t="s">
+        <v>190</v>
+      </c>
+      <c r="G56" t="s">
+        <v>190</v>
+      </c>
+      <c r="H56" t="s">
+        <v>190</v>
+      </c>
+      <c r="I56" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" t="s">
+        <v>191</v>
+      </c>
+      <c r="F57" t="s">
+        <v>191</v>
+      </c>
+      <c r="G57" t="s">
+        <v>191</v>
+      </c>
+      <c r="H57" t="s">
+        <v>191</v>
+      </c>
+      <c r="I57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" t="s">
+        <v>194</v>
+      </c>
+      <c r="D58" t="s">
+        <v>194</v>
+      </c>
+      <c r="E58" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" t="s">
+        <v>194</v>
+      </c>
+      <c r="G58" t="s">
+        <v>194</v>
+      </c>
+      <c r="H58" t="s">
+        <v>194</v>
+      </c>
+      <c r="I58" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" t="s">
+        <v>198</v>
+      </c>
+      <c r="C59" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" t="s">
+        <v>198</v>
+      </c>
+      <c r="E59" t="s">
+        <v>198</v>
+      </c>
+      <c r="F59" t="s">
+        <v>198</v>
+      </c>
+      <c r="G59" t="s">
+        <v>198</v>
+      </c>
+      <c r="H59" t="s">
+        <v>198</v>
+      </c>
+      <c r="I59" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" t="s">
+        <v>199</v>
+      </c>
+      <c r="E60" t="s">
+        <v>199</v>
+      </c>
+      <c r="F60" t="s">
+        <v>199</v>
+      </c>
+      <c r="G60" t="s">
+        <v>199</v>
+      </c>
+      <c r="H60" t="s">
+        <v>199</v>
+      </c>
+      <c r="I60" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" t="s">
+        <v>204</v>
+      </c>
+      <c r="F61" t="s">
+        <v>204</v>
+      </c>
+      <c r="G61" t="s">
+        <v>204</v>
+      </c>
+      <c r="H61" t="s">
+        <v>204</v>
+      </c>
+      <c r="I61" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" t="s">
+        <v>203</v>
+      </c>
+      <c r="C62" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" t="s">
+        <v>203</v>
+      </c>
+      <c r="E62" t="s">
+        <v>203</v>
+      </c>
+      <c r="F62" t="s">
+        <v>203</v>
+      </c>
+      <c r="G62" t="s">
+        <v>203</v>
+      </c>
+      <c r="H62" t="s">
+        <v>203</v>
+      </c>
+      <c r="I62" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" t="s">
+        <v>207</v>
+      </c>
+      <c r="C63" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" t="s">
+        <v>207</v>
+      </c>
+      <c r="E63" t="s">
+        <v>207</v>
+      </c>
+      <c r="F63" t="s">
+        <v>207</v>
+      </c>
+      <c r="G63" t="s">
+        <v>207</v>
+      </c>
+      <c r="H63" t="s">
+        <v>207</v>
+      </c>
+      <c r="I63" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64" t="s">
+        <v>212</v>
+      </c>
+      <c r="D64" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" t="s">
+        <v>211</v>
+      </c>
+      <c r="F64" t="s">
+        <v>211</v>
+      </c>
+      <c r="G64" t="s">
+        <v>211</v>
+      </c>
+      <c r="H64" t="s">
+        <v>211</v>
+      </c>
+      <c r="I64" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I4" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
v1.0.2 Fix upload bug
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A414DBB-6D31-4AD0-991E-002C8047303A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A9CE8F-D25A-40E1-8A55-C755449A2598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="250">
   <si>
     <t>id</t>
   </si>
@@ -741,6 +741,54 @@
   </si>
   <si>
     <t>สั่งซื้ออีกครั้ง</t>
+  </si>
+  <si>
+    <t>youCanCheckOrderTxt2</t>
+  </si>
+  <si>
+    <t>by input your order no.</t>
+  </si>
+  <si>
+    <t>youCanCheckOrderTxt3</t>
+  </si>
+  <si>
+    <t>and your email</t>
+  </si>
+  <si>
+    <t>โดยใส่เลขคำสั่งซื้อคือ</t>
+  </si>
+  <si>
+    <t>และอีเมล์ของท่าน</t>
+  </si>
+  <si>
+    <t>errFailToUploadQr</t>
+  </si>
+  <si>
+    <t>Fail to upload QR</t>
+  </si>
+  <si>
+    <t>ไม่สามารถสร้างคิวอาร์ได้</t>
+  </si>
+  <si>
+    <t>ไม่พบหมายเลขคำสั่งซื้อ</t>
+  </si>
+  <si>
+    <t>Invalid Order Id</t>
+  </si>
+  <si>
+    <t>No file uploaded</t>
+  </si>
+  <si>
+    <t>ไม่พบรูปหลักฐานการโอนเงิน</t>
+  </si>
+  <si>
+    <t>errFailToUploadEvidence</t>
+  </si>
+  <si>
+    <t>Fail to upload evidence</t>
+  </si>
+  <si>
+    <t>ไม่สามารถส่งหลักฐานได้</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76:I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3045,28 +3093,28 @@
         <v>220</v>
       </c>
       <c r="B67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>220</v>
+        <v>243</v>
       </c>
       <c r="D67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="E67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="F67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="G67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="H67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="I67" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -3074,10 +3122,10 @@
         <v>221</v>
       </c>
       <c r="B68" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="C68" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="D68" t="s">
         <v>221</v>
@@ -3212,6 +3260,122 @@
       </c>
       <c r="I72" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>234</v>
+      </c>
+      <c r="B73" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" t="s">
+        <v>238</v>
+      </c>
+      <c r="D73" t="s">
+        <v>235</v>
+      </c>
+      <c r="E73" t="s">
+        <v>235</v>
+      </c>
+      <c r="F73" t="s">
+        <v>235</v>
+      </c>
+      <c r="G73" t="s">
+        <v>235</v>
+      </c>
+      <c r="H73" t="s">
+        <v>235</v>
+      </c>
+      <c r="I73" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" t="s">
+        <v>239</v>
+      </c>
+      <c r="D74" t="s">
+        <v>237</v>
+      </c>
+      <c r="E74" t="s">
+        <v>237</v>
+      </c>
+      <c r="F74" t="s">
+        <v>237</v>
+      </c>
+      <c r="G74" t="s">
+        <v>237</v>
+      </c>
+      <c r="H74" t="s">
+        <v>237</v>
+      </c>
+      <c r="I74" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>240</v>
+      </c>
+      <c r="B75" t="s">
+        <v>241</v>
+      </c>
+      <c r="C75" t="s">
+        <v>242</v>
+      </c>
+      <c r="D75" t="s">
+        <v>241</v>
+      </c>
+      <c r="E75" t="s">
+        <v>241</v>
+      </c>
+      <c r="F75" t="s">
+        <v>241</v>
+      </c>
+      <c r="G75" t="s">
+        <v>241</v>
+      </c>
+      <c r="H75" t="s">
+        <v>241</v>
+      </c>
+      <c r="I75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>247</v>
+      </c>
+      <c r="B76" t="s">
+        <v>248</v>
+      </c>
+      <c r="C76" t="s">
+        <v>249</v>
+      </c>
+      <c r="D76" t="s">
+        <v>248</v>
+      </c>
+      <c r="E76" t="s">
+        <v>248</v>
+      </c>
+      <c r="F76" t="s">
+        <v>248</v>
+      </c>
+      <c r="G76" t="s">
+        <v>248</v>
+      </c>
+      <c r="H76" t="s">
+        <v>248</v>
+      </c>
+      <c r="I76" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V1.0.5 Done admin photo
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293FB5AD-E6FE-4EAC-A9CA-AC624E2BB1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960FAC20-31BF-4214-A8AA-0828A1FC45B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="348">
   <si>
     <t>id</t>
   </si>
@@ -1026,6 +1026,63 @@
   </si>
   <si>
     <t>แก้ไขครั้งล่าสุด</t>
+  </si>
+  <si>
+    <t>emsTracking</t>
+  </si>
+  <si>
+    <t>EMS Tracking</t>
+  </si>
+  <si>
+    <t>หมายเลขติดตามพัสดุ</t>
+  </si>
+  <si>
+    <t>mailerTextUpdateOrder1</t>
+  </si>
+  <si>
+    <t>mailerTextUpdateOrder2</t>
+  </si>
+  <si>
+    <t>mailerTextUpdateOrder3</t>
+  </si>
+  <si>
+    <t>mailerSubjectUpdateOrder</t>
+  </si>
+  <si>
+    <t>[ICMM2025] Your order has been updated!...</t>
+  </si>
+  <si>
+    <t>We have updated your order status or detail.</t>
+  </si>
+  <si>
+    <t>[ICMM2025] คำสั่งซื้อของท่านมีการเปลี่ยนสถานะหรือแก้ไข…</t>
+  </si>
+  <si>
+    <t>เราได้ทำการเปลี่ยนแปลงสถานะหรือรายละเอียดคำสั่งซื้อของท่าน</t>
+  </si>
+  <si>
+    <t>[ICMM2025] คำสั่งซื้อของท่านมีการเปลี่ยนสถานะ…</t>
+  </si>
+  <si>
+    <t>mailerTextFwdOrder1</t>
+  </si>
+  <si>
+    <t>mailerTextFwdOrder3</t>
+  </si>
+  <si>
+    <t>mailerTextFwdOrder2</t>
+  </si>
+  <si>
+    <t>mailerSubjectFwdOrder</t>
+  </si>
+  <si>
+    <t>[ICMM2025] Your order has changed status!...</t>
+  </si>
+  <si>
+    <t>We have moved your order to the next state.</t>
+  </si>
+  <si>
+    <t>คำสั่งซื้อของท่านถูกทำเดินการไปยังสถานะถัดไป</t>
   </si>
 </sst>
 </file>
@@ -1403,15 +1460,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101:I102"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104:I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="3" max="3" width="47.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4370,6 +4428,267 @@
       </c>
       <c r="I102" t="s">
         <v>326</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>329</v>
+      </c>
+      <c r="B103" t="s">
+        <v>330</v>
+      </c>
+      <c r="C103" t="s">
+        <v>331</v>
+      </c>
+      <c r="D103" t="s">
+        <v>330</v>
+      </c>
+      <c r="E103" t="s">
+        <v>330</v>
+      </c>
+      <c r="F103" t="s">
+        <v>330</v>
+      </c>
+      <c r="G103" t="s">
+        <v>330</v>
+      </c>
+      <c r="H103" t="s">
+        <v>330</v>
+      </c>
+      <c r="I103" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>332</v>
+      </c>
+      <c r="B104" t="s">
+        <v>337</v>
+      </c>
+      <c r="C104" t="s">
+        <v>339</v>
+      </c>
+      <c r="D104" t="s">
+        <v>337</v>
+      </c>
+      <c r="E104" t="s">
+        <v>337</v>
+      </c>
+      <c r="F104" t="s">
+        <v>337</v>
+      </c>
+      <c r="G104" t="s">
+        <v>337</v>
+      </c>
+      <c r="H104" t="s">
+        <v>337</v>
+      </c>
+      <c r="I104" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>333</v>
+      </c>
+      <c r="B105" t="s">
+        <v>266</v>
+      </c>
+      <c r="C105" t="s">
+        <v>270</v>
+      </c>
+      <c r="D105" t="s">
+        <v>266</v>
+      </c>
+      <c r="E105" t="s">
+        <v>266</v>
+      </c>
+      <c r="F105" t="s">
+        <v>266</v>
+      </c>
+      <c r="G105" t="s">
+        <v>266</v>
+      </c>
+      <c r="H105" t="s">
+        <v>266</v>
+      </c>
+      <c r="I105" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>334</v>
+      </c>
+      <c r="B106" t="s">
+        <v>267</v>
+      </c>
+      <c r="C106" t="s">
+        <v>271</v>
+      </c>
+      <c r="D106" t="s">
+        <v>267</v>
+      </c>
+      <c r="E106" t="s">
+        <v>267</v>
+      </c>
+      <c r="F106" t="s">
+        <v>267</v>
+      </c>
+      <c r="G106" t="s">
+        <v>267</v>
+      </c>
+      <c r="H106" t="s">
+        <v>267</v>
+      </c>
+      <c r="I106" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>335</v>
+      </c>
+      <c r="B107" t="s">
+        <v>336</v>
+      </c>
+      <c r="C107" t="s">
+        <v>338</v>
+      </c>
+      <c r="D107" t="s">
+        <v>336</v>
+      </c>
+      <c r="E107" t="s">
+        <v>336</v>
+      </c>
+      <c r="F107" t="s">
+        <v>336</v>
+      </c>
+      <c r="G107" t="s">
+        <v>336</v>
+      </c>
+      <c r="H107" t="s">
+        <v>336</v>
+      </c>
+      <c r="I107" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>341</v>
+      </c>
+      <c r="B108" t="s">
+        <v>346</v>
+      </c>
+      <c r="C108" t="s">
+        <v>347</v>
+      </c>
+      <c r="D108" t="s">
+        <v>346</v>
+      </c>
+      <c r="E108" t="s">
+        <v>346</v>
+      </c>
+      <c r="F108" t="s">
+        <v>346</v>
+      </c>
+      <c r="G108" t="s">
+        <v>346</v>
+      </c>
+      <c r="H108" t="s">
+        <v>346</v>
+      </c>
+      <c r="I108" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>343</v>
+      </c>
+      <c r="B109" t="s">
+        <v>266</v>
+      </c>
+      <c r="C109" t="s">
+        <v>270</v>
+      </c>
+      <c r="D109" t="s">
+        <v>266</v>
+      </c>
+      <c r="E109" t="s">
+        <v>266</v>
+      </c>
+      <c r="F109" t="s">
+        <v>266</v>
+      </c>
+      <c r="G109" t="s">
+        <v>266</v>
+      </c>
+      <c r="H109" t="s">
+        <v>266</v>
+      </c>
+      <c r="I109" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>342</v>
+      </c>
+      <c r="B110" t="s">
+        <v>267</v>
+      </c>
+      <c r="C110" t="s">
+        <v>271</v>
+      </c>
+      <c r="D110" t="s">
+        <v>267</v>
+      </c>
+      <c r="E110" t="s">
+        <v>267</v>
+      </c>
+      <c r="F110" t="s">
+        <v>267</v>
+      </c>
+      <c r="G110" t="s">
+        <v>267</v>
+      </c>
+      <c r="H110" t="s">
+        <v>267</v>
+      </c>
+      <c r="I110" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>344</v>
+      </c>
+      <c r="B111" t="s">
+        <v>345</v>
+      </c>
+      <c r="C111" t="s">
+        <v>340</v>
+      </c>
+      <c r="D111" t="s">
+        <v>345</v>
+      </c>
+      <c r="E111" t="s">
+        <v>345</v>
+      </c>
+      <c r="F111" t="s">
+        <v>345</v>
+      </c>
+      <c r="G111" t="s">
+        <v>345</v>
+      </c>
+      <c r="H111" t="s">
+        <v>345</v>
+      </c>
+      <c r="I111" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1.7 update admin new address
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1411EA9-787E-410D-AF90-12623DF54A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6177B1C9-D00D-4B90-83C3-6D36A0322485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -3316,12 +3316,6 @@
     <t>Your order has been delivered. Please check your delivery status from tracking number.</t>
   </si>
   <si>
-    <t>Created at (at เวลา, on วันที่ เอาแบบใด)</t>
-  </si>
-  <si>
-    <t>Updated (at เวลา, on วันที่ เอาแบบใด)</t>
-  </si>
-  <si>
     <t>EMS tracking number</t>
   </si>
   <si>
@@ -3446,6 +3440,12 @@
   </si>
   <si>
     <t>หมวกวิ่ง + ผ้าบัฟ รุ่น Coolnet UV + กางเกงวิ่งขาสั้นหญิง 3 นิ้ว</t>
+  </si>
+  <si>
+    <t>Created at</t>
+  </si>
+  <si>
+    <t>Updated at</t>
   </si>
 </sst>
 </file>
@@ -3825,8 +3825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
   <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4137,7 +4137,7 @@
         <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C28" t="s">
         <v>1044</v>
@@ -4159,10 +4159,10 @@
         <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C30" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -4181,10 +4181,10 @@
         <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C32" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -4192,10 +4192,10 @@
         <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C33" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -4203,10 +4203,10 @@
         <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C34" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -4214,10 +4214,10 @@
         <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="C35" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -4225,10 +4225,10 @@
         <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C36" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -4236,10 +4236,10 @@
         <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="C37" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -4247,10 +4247,10 @@
         <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C38" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -4258,10 +4258,10 @@
         <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C39" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -4269,10 +4269,10 @@
         <v>1028</v>
       </c>
       <c r="B40" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="C40" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -4280,10 +4280,10 @@
         <v>1029</v>
       </c>
       <c r="B41" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="C41" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -4984,7 +4984,7 @@
         <v>313</v>
       </c>
       <c r="B105" t="s">
-        <v>1091</v>
+        <v>1131</v>
       </c>
       <c r="C105" t="s">
         <v>317</v>
@@ -4995,7 +4995,7 @@
         <v>314</v>
       </c>
       <c r="B106" t="s">
-        <v>1092</v>
+        <v>1132</v>
       </c>
       <c r="C106" t="s">
         <v>318</v>
@@ -5006,7 +5006,7 @@
         <v>319</v>
       </c>
       <c r="B107" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="C107" t="s">
         <v>321</v>
@@ -5017,7 +5017,7 @@
         <v>322</v>
       </c>
       <c r="B108" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C108" t="s">
         <v>329</v>
@@ -5028,7 +5028,7 @@
         <v>323</v>
       </c>
       <c r="B109" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C109" t="s">
         <v>265</v>
@@ -5050,7 +5050,7 @@
         <v>325</v>
       </c>
       <c r="B111" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C111" t="s">
         <v>1009</v>
@@ -5064,7 +5064,7 @@
         <v>336</v>
       </c>
       <c r="C112" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -5072,7 +5072,7 @@
         <v>333</v>
       </c>
       <c r="B113" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C113" t="s">
         <v>265</v>
@@ -5094,7 +5094,7 @@
         <v>334</v>
       </c>
       <c r="B115" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="C115" t="s">
         <v>1010</v>
@@ -5138,7 +5138,7 @@
         <v>944</v>
       </c>
       <c r="B119" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C119" t="s">
         <v>946</v>
@@ -5149,7 +5149,7 @@
         <v>947</v>
       </c>
       <c r="B120" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="C120" t="s">
         <v>949</v>
@@ -5182,7 +5182,7 @@
         <v>956</v>
       </c>
       <c r="B123" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="C123" t="s">
         <v>255</v>
@@ -5193,10 +5193,10 @@
         <v>962</v>
       </c>
       <c r="B124" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C124" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -5204,7 +5204,7 @@
         <v>963</v>
       </c>
       <c r="B125" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C125" t="s">
         <v>265</v>
@@ -5226,7 +5226,7 @@
         <v>967</v>
       </c>
       <c r="B127" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C127" t="s">
         <v>969</v>
@@ -5248,10 +5248,10 @@
         <v>975</v>
       </c>
       <c r="B129" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C129" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -5281,7 +5281,7 @@
         <v>1011</v>
       </c>
       <c r="B132" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C132" t="s">
         <v>1012</v>
@@ -5292,7 +5292,7 @@
         <v>1013</v>
       </c>
       <c r="B133" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C133" t="s">
         <v>1014</v>
@@ -5325,7 +5325,7 @@
         <v>1021</v>
       </c>
       <c r="B136" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C136" t="s">
         <v>1022</v>
@@ -5343,8 +5343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08623EB8-71BE-44FC-9615-87E1DDBD6EF4}">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C39"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
v1.1.8 Done change email and acc
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC180DB-3671-477A-BC26-4528097B6CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E882E4A1-E8C4-4E92-9C63-36CB440776B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="1155">
   <si>
     <t>id</t>
   </si>
@@ -3059,12 +3059,6 @@
   </si>
   <si>
     <t>ชำระเงินไม่สำเร็จ</t>
-  </si>
-  <si>
-    <t>Please create new order.</t>
-  </si>
-  <si>
-    <t>กรุณาสร้างคำสั่งซื้อใหม่อีกครั้ง</t>
   </si>
   <si>
     <t>ขอบคุณที่เลือกซื้อสินค้ากับเรา</t>
@@ -3479,6 +3473,63 @@
 +ออกแบบมาสำหรับทุกกิจกรรม ไม่ว่าจะเป็นการซ้อม การลงแข่งขัน หรือการออกกำลังกายประเภทอื่นๆ
 +เนื้อผ้าด้านนอกมีน้ำหนักเบา ระบายอากาศดี และแห้งไว เนื้อผ้าด้านในมีความยืดหยุ่น กระชับ
 +มาพร้อมกับกระเป๋ารอบตัว ซ้าย ขวา หน้า หลัง</t>
+  </si>
+  <si>
+    <t>Address must be between 1 and 400 characters</t>
+  </si>
+  <si>
+    <t>errAddress1to400</t>
+  </si>
+  <si>
+    <t>deliveryWithinThailandOnly</t>
+  </si>
+  <si>
+    <t>จัดส่งภายในประเทศเท่านั้น</t>
+  </si>
+  <si>
+    <t>Delivery within Thailand only.</t>
+  </si>
+  <si>
+    <t>Please finish payment or create new order.</t>
+  </si>
+  <si>
+    <t>กรุณาชำระค่าสินค้าหรือสร้างคำสั่งซื้อใหม่</t>
+  </si>
+  <si>
+    <t>orPayByQr</t>
+  </si>
+  <si>
+    <t>หรือชำระผ่าน QR Code</t>
+  </si>
+  <si>
+    <t>or pay via QR code.</t>
+  </si>
+  <si>
+    <t>orderDetail</t>
+  </si>
+  <si>
+    <t>Order Detail</t>
+  </si>
+  <si>
+    <t>รายละเอียดสินค้า</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>ชื่อสินค้า</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>จำนวน</t>
   </si>
 </sst>
 </file>
@@ -3859,10 +3910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
-  <dimension ref="A1:C136"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142:C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3942,10 +3993,10 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C7" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3953,7 +4004,7 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C8" t="s">
         <v>50</v>
@@ -3975,10 +4026,10 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C10" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -4008,10 +4059,10 @@
         <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C13" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -4041,7 +4092,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C16" t="s">
         <v>73</v>
@@ -4063,7 +4114,7 @@
         <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C18" t="s">
         <v>79</v>
@@ -4077,7 +4128,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -4096,10 +4147,10 @@
         <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C21" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -4118,7 +4169,7 @@
         <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C23" t="s">
         <v>988</v>
@@ -4129,7 +4180,7 @@
         <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="C24" t="s">
         <v>99</v>
@@ -4151,7 +4202,7 @@
         <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C26" t="s">
         <v>100</v>
@@ -4173,10 +4224,10 @@
         <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C28" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -4184,7 +4235,7 @@
         <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C29" t="s">
         <v>108</v>
@@ -4195,10 +4246,10 @@
         <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="C30" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -4206,10 +4257,10 @@
         <v>134</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -4217,10 +4268,10 @@
         <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C32" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -4228,10 +4279,10 @@
         <v>135</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -4239,10 +4290,10 @@
         <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C34" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="144" x14ac:dyDescent="0.3">
@@ -4250,10 +4301,10 @@
         <v>136</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -4261,10 +4312,10 @@
         <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C36" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="144" x14ac:dyDescent="0.3">
@@ -4272,10 +4323,10 @@
         <v>137</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -4283,10 +4334,10 @@
         <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C38" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -4294,32 +4345,32 @@
         <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C39" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B40" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C40" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B41" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="C41" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -4349,7 +4400,7 @@
         <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C44" t="s">
         <v>147</v>
@@ -4360,10 +4411,10 @@
         <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C45" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -4382,7 +4433,7 @@
         <v>151</v>
       </c>
       <c r="B47" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C47" t="s">
         <v>154</v>
@@ -4393,7 +4444,7 @@
         <v>156</v>
       </c>
       <c r="B48" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C48" t="s">
         <v>158</v>
@@ -4404,7 +4455,7 @@
         <v>160</v>
       </c>
       <c r="B49" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C49" t="s">
         <v>162</v>
@@ -4418,7 +4469,7 @@
         <v>163</v>
       </c>
       <c r="C50" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -4440,15 +4491,15 @@
         <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B53" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C53" t="s">
         <v>171</v>
@@ -4456,915 +4507,981 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1025</v>
+        <v>1137</v>
       </c>
       <c r="B54" t="s">
-        <v>1026</v>
+        <v>1136</v>
       </c>
       <c r="C54" t="s">
-        <v>1027</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>1023</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>1024</v>
       </c>
       <c r="C55" t="s">
-        <v>992</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
+        <v>992</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
-        <v>993</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B58" t="s">
-        <v>1049</v>
+        <v>180</v>
       </c>
       <c r="C58" t="s">
-        <v>1050</v>
+        <v>993</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>1047</v>
       </c>
       <c r="C59" t="s">
-        <v>185</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>994</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C62" t="s">
-        <v>193</v>
+        <v>995</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B63" t="s">
-        <v>1122</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>996</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B64" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="C64" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B65" t="s">
-        <v>1051</v>
+        <v>1121</v>
       </c>
       <c r="C65" t="s">
-        <v>1052</v>
+        <v>997</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B66" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="C66" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B67" t="s">
-        <v>1124</v>
+        <v>1051</v>
       </c>
       <c r="C67" t="s">
-        <v>1125</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>1055</v>
+        <v>1122</v>
       </c>
       <c r="C68" t="s">
-        <v>998</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>1053</v>
       </c>
       <c r="C69" t="s">
-        <v>213</v>
+        <v>998</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B70" t="s">
-        <v>1056</v>
+        <v>214</v>
       </c>
       <c r="C70" t="s">
-        <v>1057</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B72" t="s">
-        <v>243</v>
+        <v>1056</v>
       </c>
       <c r="C72" t="s">
-        <v>1059</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B73" t="s">
-        <v>1060</v>
+        <v>243</v>
       </c>
       <c r="C73" t="s">
-        <v>999</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="C74" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B75" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C75" t="s">
-        <v>1063</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B76" t="s">
-        <v>230</v>
+        <v>1060</v>
       </c>
       <c r="C76" t="s">
-        <v>231</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B77" t="s">
-        <v>1064</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>1065</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B78" t="s">
-        <v>235</v>
+        <v>1062</v>
       </c>
       <c r="C78" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B79" t="s">
-        <v>1067</v>
+        <v>235</v>
       </c>
       <c r="C79" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B80" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="C80" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="C81" t="s">
-        <v>252</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="C82" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B83" t="s">
-        <v>1001</v>
+        <v>1070</v>
       </c>
       <c r="C83" t="s">
-        <v>1002</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B84" t="s">
-        <v>261</v>
+        <v>1001</v>
       </c>
       <c r="C84" t="s">
-        <v>264</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B85" t="s">
-        <v>1073</v>
+        <v>261</v>
       </c>
       <c r="C85" t="s">
-        <v>1003</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>1071</v>
       </c>
       <c r="C86" t="s">
-        <v>265</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C87" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C88" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B89" t="s">
-        <v>1004</v>
+        <v>259</v>
       </c>
       <c r="C89" t="s">
-        <v>1126</v>
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B90" t="s">
-        <v>274</v>
+        <v>1004</v>
       </c>
       <c r="C90" t="s">
-        <v>273</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B91" t="s">
-        <v>1074</v>
+        <v>274</v>
       </c>
       <c r="C91" t="s">
-        <v>1075</v>
+        <v>273</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B92" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C92" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B93" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="C93" t="s">
-        <v>1005</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B94" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="C94" t="s">
-        <v>292</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>287</v>
+        <v>1077</v>
       </c>
       <c r="C95" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B96" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C96" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B97" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C97" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B98" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C98" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B99" t="s">
-        <v>1006</v>
+        <v>290</v>
       </c>
       <c r="C99" t="s">
-        <v>1007</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B100" t="s">
-        <v>1080</v>
+        <v>1141</v>
       </c>
       <c r="C100" t="s">
-        <v>308</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B101" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C101" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B102" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C102" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B103" t="s">
-        <v>306</v>
+        <v>1080</v>
       </c>
       <c r="C103" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B104" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C104" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="B105" t="s">
-        <v>1114</v>
+        <v>307</v>
       </c>
       <c r="C105" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B106" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="C106" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B107" t="s">
-        <v>1083</v>
+        <v>1113</v>
       </c>
       <c r="C107" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B108" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="C108" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B109" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="C109" t="s">
-        <v>265</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B110" t="s">
-        <v>263</v>
+        <v>1083</v>
       </c>
       <c r="C110" t="s">
-        <v>1008</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B111" t="s">
-        <v>1086</v>
+        <v>263</v>
       </c>
       <c r="C111" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B112" t="s">
-        <v>336</v>
+        <v>1084</v>
       </c>
       <c r="C112" t="s">
-        <v>1087</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B113" t="s">
+        <v>336</v>
+      </c>
+      <c r="C113" t="s">
         <v>1085</v>
-      </c>
-      <c r="C113" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B114" t="s">
-        <v>263</v>
+        <v>1083</v>
       </c>
       <c r="C114" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B115" t="s">
-        <v>1088</v>
+        <v>263</v>
       </c>
       <c r="C115" t="s">
-        <v>1010</v>
+        <v>266</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>935</v>
+        <v>334</v>
       </c>
       <c r="B116" t="s">
-        <v>936</v>
+        <v>1086</v>
       </c>
       <c r="C116" t="s">
-        <v>937</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B117" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C117" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="B118" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="C118" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B119" t="s">
-        <v>1089</v>
+        <v>942</v>
       </c>
       <c r="C119" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="B120" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="C120" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="B121" t="s">
-        <v>951</v>
+        <v>1088</v>
       </c>
       <c r="C121" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="B122" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="C122" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="B123" t="s">
-        <v>1127</v>
+        <v>955</v>
       </c>
       <c r="C123" t="s">
-        <v>1002</v>
+        <v>954</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="B124" t="s">
-        <v>1091</v>
+        <v>1125</v>
       </c>
       <c r="C124" t="s">
-        <v>1092</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B125" t="s">
-        <v>1085</v>
+        <v>1089</v>
       </c>
       <c r="C125" t="s">
-        <v>265</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B126" t="s">
-        <v>263</v>
+        <v>1083</v>
       </c>
       <c r="C126" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B127" t="s">
-        <v>1093</v>
+        <v>263</v>
       </c>
       <c r="C127" t="s">
-        <v>969</v>
+        <v>266</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="B128" t="s">
-        <v>971</v>
+        <v>1091</v>
       </c>
       <c r="C128" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>975</v>
+        <v>970</v>
       </c>
       <c r="B129" t="s">
-        <v>1094</v>
+        <v>971</v>
       </c>
       <c r="C129" t="s">
-        <v>1095</v>
+        <v>972</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="B130" t="s">
-        <v>979</v>
+        <v>1092</v>
       </c>
       <c r="C130" t="s">
-        <v>980</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="B131" t="s">
-        <v>984</v>
+        <v>979</v>
       </c>
       <c r="C131" t="s">
-        <v>985</v>
+        <v>980</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>1011</v>
+        <v>983</v>
       </c>
       <c r="B132" t="s">
-        <v>1097</v>
+        <v>984</v>
       </c>
       <c r="C132" t="s">
-        <v>1012</v>
+        <v>985</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="B133" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="C133" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="B134" t="s">
-        <v>1016</v>
+        <v>1096</v>
       </c>
       <c r="C134" t="s">
-        <v>1017</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>1018</v>
+        <v>1013</v>
       </c>
       <c r="B135" t="s">
-        <v>1019</v>
+        <v>1014</v>
       </c>
       <c r="C135" t="s">
-        <v>1020</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>1021</v>
+        <v>1016</v>
       </c>
       <c r="B136" t="s">
-        <v>1099</v>
+        <v>1017</v>
       </c>
       <c r="C136" t="s">
-        <v>1022</v>
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C138" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C139" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C140" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C141" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1154</v>
       </c>
     </row>
   </sheetData>
@@ -5377,10 +5494,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08623EB8-71BE-44FC-9615-87E1DDBD6EF4}">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C129" sqref="A129:C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9102,6 +9219,17 @@
         <v>984</v>
       </c>
     </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1154</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I4" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.2.0 add new product and disable option
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -2,22 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F8E79A-57FB-4496-B0DA-BEF9D2BC93DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC7A30D-AF4E-4953-A4FA-251022401FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
-    <sheet name="BAK_20250814" sheetId="3" r:id="rId2"/>
+    <sheet name="BAK_20250916" sheetId="4" r:id="rId2"/>
+    <sheet name="BAK_20250814" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BAK_20250814!$A$1:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">BAK_20250814!$A$1:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BAK_20250916!$A$1:$C$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1.0000000000000001E-5" calcOnSave="0"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="1171">
   <si>
     <t>id</t>
   </si>
@@ -3536,6 +3538,48 @@
   </si>
   <si>
     <t>Intania Runner</t>
+  </si>
+  <si>
+    <t>Running Set (Men) - Black Cap</t>
+  </si>
+  <si>
+    <t>เซ็ตสำหรับนักวิ่งชาย - หมวกสีดำ</t>
+  </si>
+  <si>
+    <t>Running Set (Women) - Black Cap</t>
+  </si>
+  <si>
+    <t>เซ็ทสำหรับนักวิ่งหญิง - หมวกสีดำ</t>
+  </si>
+  <si>
+    <t>prod7Name</t>
+  </si>
+  <si>
+    <t>Running Set (Men) - White Cap</t>
+  </si>
+  <si>
+    <t>เซ็ตสำหรับนักวิ่งชาย - หมวกสีขาว</t>
+  </si>
+  <si>
+    <t>prod7Detail</t>
+  </si>
+  <si>
+    <t>Running Cap + Original BUFF® Coolnet UV + Men’s 3" Running Shorts</t>
+  </si>
+  <si>
+    <t>หมวกวิ่ง + ผ้าบัฟ รุ่น Coolnet UV + กางเกงวิ่งขาสั้นชาย 3 นิ้ว</t>
+  </si>
+  <si>
+    <t>prod8Name</t>
+  </si>
+  <si>
+    <t>Running Set (Women) - White Cap</t>
+  </si>
+  <si>
+    <t>เซ็ทสำหรับนักวิ่งหญิง - หมวกสีขาว</t>
+  </si>
+  <si>
+    <t>prod8Detail</t>
   </si>
 </sst>
 </file>
@@ -3919,10 +3963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
-  <dimension ref="A1:C142"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4343,10 +4388,10 @@
         <v>113</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1099</v>
+        <v>1157</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1100</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -4365,10 +4410,10 @@
         <v>1023</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1102</v>
+        <v>1159</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1103</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -4384,799 +4429,799 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>139</v>
+        <v>1161</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>140</v>
+        <v>1162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>141</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>1164</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>143</v>
+        <v>1165</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>1167</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1040</v>
+        <v>1168</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>147</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>1170</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1109</v>
+        <v>1119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1111</v>
+        <v>143</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1042</v>
+        <v>1109</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>162</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1043</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>167</v>
+        <v>1111</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>170</v>
+        <v>1041</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1112</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1018</v>
+        <v>160</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1019</v>
+        <v>1042</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1129</v>
+        <v>164</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1128</v>
+        <v>163</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>171</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1020</v>
+        <v>166</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1021</v>
+        <v>167</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1022</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>992</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>1018</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>174</v>
+        <v>1019</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>1129</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>180</v>
+        <v>1128</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>993</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>179</v>
+        <v>1020</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1044</v>
+        <v>1021</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1045</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>185</v>
+        <v>992</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>994</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>193</v>
+        <v>1044</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>193</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1113</v>
+        <v>186</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>996</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1114</v>
+        <v>189</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1046</v>
+        <v>190</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1047</v>
+        <v>995</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1048</v>
+        <v>193</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1049</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1116</v>
+        <v>996</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1050</v>
+        <v>1114</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>214</v>
+        <v>1046</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>213</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1053</v>
+        <v>1115</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>241</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>243</v>
+        <v>1050</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1054</v>
+        <v>998</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1055</v>
+        <v>214</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>999</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1149</v>
+        <v>1051</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1150</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1057</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>231</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1059</v>
+        <v>999</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>235</v>
+        <v>1149</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1060</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1061</v>
+        <v>1056</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1062</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1063</v>
+        <v>230</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1064</v>
+        <v>231</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1065</v>
+        <v>1058</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>252</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1066</v>
+        <v>235</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>253</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1000</v>
+        <v>1061</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1001</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>261</v>
+        <v>1063</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1155</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1151</v>
+        <v>1065</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1152</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>262</v>
+        <v>1066</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>263</v>
+        <v>1000</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>266</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>268</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1067</v>
+        <v>263</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1068</v>
+        <v>266</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>1069</v>
+        <v>259</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1070</v>
+        <v>268</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1071</v>
+        <v>1156</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1002</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>1072</v>
+        <v>274</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>287</v>
+        <v>1067</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>293</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>288</v>
+        <v>1069</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>294</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>289</v>
+        <v>1071</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>295</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>290</v>
+        <v>1072</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>1133</v>
+        <v>287</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1134</v>
+        <v>293</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>1073</v>
+        <v>288</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1154</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>1074</v>
+        <v>289</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1075</v>
+        <v>290</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>306</v>
+        <v>1133</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>311</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>307</v>
+        <v>1073</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>312</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1105</v>
+        <v>1074</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1106</v>
+        <v>1075</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1076</v>
+        <v>306</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>1077</v>
+        <v>307</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1078</v>
+        <v>1105</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>265</v>
+        <v>317</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>263</v>
+        <v>1106</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1003</v>
+        <v>318</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>1004</v>
+        <v>321</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>336</v>
+        <v>1077</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>1080</v>
+        <v>329</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>1078</v>
@@ -5187,309 +5232,353 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>263</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>266</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>935</v>
+        <v>331</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>936</v>
+        <v>336</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>937</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>938</v>
+        <v>333</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>939</v>
+        <v>1078</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>940</v>
+        <v>265</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>941</v>
+        <v>332</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>942</v>
+        <v>263</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>943</v>
+        <v>266</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>944</v>
+        <v>334</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>946</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>947</v>
+        <v>935</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1083</v>
+        <v>936</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>955</v>
+        <v>942</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>954</v>
+        <v>943</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1117</v>
+        <v>1082</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>1001</v>
+        <v>946</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>962</v>
+        <v>947</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1085</v>
+        <v>949</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>963</v>
+        <v>950</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>1078</v>
+        <v>951</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>265</v>
+        <v>952</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>964</v>
+        <v>953</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>263</v>
+        <v>955</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>266</v>
+        <v>954</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>967</v>
+        <v>956</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1086</v>
+        <v>1117</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>969</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>970</v>
+        <v>962</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>971</v>
+        <v>1084</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>972</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>975</v>
+        <v>963</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1087</v>
+        <v>1078</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>1088</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>978</v>
+        <v>964</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>979</v>
+        <v>263</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>980</v>
+        <v>266</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>983</v>
+        <v>967</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>984</v>
+        <v>1086</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>985</v>
+        <v>969</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>1006</v>
+        <v>970</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1090</v>
+        <v>971</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>1007</v>
+        <v>972</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>1008</v>
+        <v>975</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1009</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>1010</v>
+        <v>978</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1011</v>
+        <v>979</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1012</v>
+        <v>980</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>1013</v>
+        <v>983</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1014</v>
+        <v>984</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1015</v>
+        <v>985</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>1016</v>
+        <v>1006</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1017</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1130</v>
+        <v>1008</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1132</v>
+        <v>1091</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1131</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>1135</v>
+        <v>1010</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>1137</v>
+        <v>1011</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1136</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>1138</v>
+        <v>1013</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>1139</v>
+        <v>1014</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>1140</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1141</v>
+        <v>1016</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1143</v>
+        <v>1092</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1142</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>1144</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>1145</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>1146</v>
       </c>
     </row>
@@ -5502,11 +5591,1596 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E473FA-375A-45CE-B9D9-17513763A224}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C142"/>
+  <sheetViews>
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="42.5546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>178</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>205</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>209</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>222</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>228</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>229</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>232</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>234</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>238</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>245</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>250</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>251</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>256</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>271</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>269</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>270</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>257</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>258</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>272</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>275</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>278</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>281</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>282</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>283</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>285</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>286</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>297</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>298</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>299</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>300</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>301</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>302</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>313</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>319</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>322</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>323</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>324</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>325</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>331</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>333</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>332</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>334</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>935</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>938</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>941</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>944</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>947</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>950</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>953</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>956</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>962</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>963</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>964</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>967</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>970</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>975</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>978</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>983</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C4" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08623EB8-71BE-44FC-9615-87E1DDBD6EF4}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C129" sqref="A129:C129"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
v1.2.1 add product 9 & 10
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC7A30D-AF4E-4953-A4FA-251022401FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D99F5DC-12FE-4384-935D-99BEBFB4B6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1183">
   <si>
     <t>id</t>
   </si>
@@ -3580,6 +3580,42 @@
   </si>
   <si>
     <t>prod8Detail</t>
+  </si>
+  <si>
+    <t>prod9Name</t>
+  </si>
+  <si>
+    <t>prod9Detail</t>
+  </si>
+  <si>
+    <t>prod10Name</t>
+  </si>
+  <si>
+    <t>prod10Detail</t>
+  </si>
+  <si>
+    <t>Buff + Short (Men) Set</t>
+  </si>
+  <si>
+    <t>เซ็ตผ้าบัฟและกางเกงวิ่ง (ชาย)</t>
+  </si>
+  <si>
+    <t>Original BUFF® Coolnet UV + Men’s 3" Running Shorts</t>
+  </si>
+  <si>
+    <t>ผ้าบัฟ รุ่น Coolnet UV + กางเกงวิ่งขาสั้นชาย 3 นิ้ว</t>
+  </si>
+  <si>
+    <t>Buff + Short (Women) Set</t>
+  </si>
+  <si>
+    <t>เซ็ตผ้าบัฟและกางเกงวิ่ง (หญิง)</t>
+  </si>
+  <si>
+    <t>Original BUFF® Coolnet UV + Women's 5" Running Shorts</t>
+  </si>
+  <si>
+    <t>ผ้าบัฟ รุ่น Coolnet UV + กางเกงวิ่งขาสั้นหญิง 3 นิ้ว</t>
   </si>
 </sst>
 </file>
@@ -3964,10 +4000,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4473,799 +4509,799 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>1171</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>140</v>
+        <v>1175</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>141</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>1172</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>143</v>
+        <v>1177</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>144</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>1173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1040</v>
+        <v>1179</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>147</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>1174</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1109</v>
+        <v>1181</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1110</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1111</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1042</v>
+        <v>1109</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>162</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1043</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>167</v>
+        <v>1111</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>170</v>
+        <v>1041</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1112</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1018</v>
+        <v>160</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1019</v>
+        <v>1042</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1129</v>
+        <v>164</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1128</v>
+        <v>163</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>171</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1020</v>
+        <v>166</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1021</v>
+        <v>167</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1022</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>992</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>1018</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>174</v>
+        <v>1019</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>1129</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>180</v>
+        <v>1128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>993</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>1020</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1044</v>
+        <v>1021</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1045</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>185</v>
+        <v>992</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>994</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>193</v>
+        <v>1044</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>193</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1113</v>
+        <v>186</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>996</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1114</v>
+        <v>189</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1046</v>
+        <v>190</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1047</v>
+        <v>995</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1048</v>
+        <v>193</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1049</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1116</v>
+        <v>996</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1050</v>
+        <v>1114</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>214</v>
+        <v>1046</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>213</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1053</v>
+        <v>1115</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>241</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>243</v>
+        <v>1050</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1054</v>
+        <v>998</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1055</v>
+        <v>214</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>999</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1149</v>
+        <v>1051</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1150</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1057</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>231</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1059</v>
+        <v>999</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>235</v>
+        <v>1149</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1060</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1061</v>
+        <v>1056</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1062</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1063</v>
+        <v>230</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1064</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1065</v>
+        <v>1058</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>252</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1066</v>
+        <v>235</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>253</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1000</v>
+        <v>1061</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1001</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>261</v>
+        <v>1063</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1155</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1151</v>
+        <v>1065</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1152</v>
+        <v>252</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>262</v>
+        <v>1066</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>263</v>
+        <v>1000</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>266</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>268</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1067</v>
+        <v>263</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1068</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>1069</v>
+        <v>259</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1070</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>1071</v>
+        <v>1156</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1002</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>1072</v>
+        <v>274</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>287</v>
+        <v>1067</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>293</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>288</v>
+        <v>1069</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>294</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>289</v>
+        <v>1071</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>295</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>290</v>
+        <v>1072</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1133</v>
+        <v>287</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1134</v>
+        <v>293</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>1073</v>
+        <v>288</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1154</v>
+        <v>294</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1074</v>
+        <v>289</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1075</v>
+        <v>290</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>306</v>
+        <v>1133</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>311</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>307</v>
+        <v>1073</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>312</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>1105</v>
+        <v>1074</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>1106</v>
+        <v>1075</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1076</v>
+        <v>306</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>1077</v>
+        <v>307</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>1078</v>
+        <v>1105</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>265</v>
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>263</v>
+        <v>1106</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1003</v>
+        <v>318</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1004</v>
+        <v>321</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>336</v>
+        <v>1077</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1080</v>
+        <v>329</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>1078</v>
@@ -5276,309 +5312,353 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>263</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>266</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>935</v>
+        <v>331</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>936</v>
+        <v>336</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>937</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>938</v>
+        <v>333</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>939</v>
+        <v>1078</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>940</v>
+        <v>265</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>941</v>
+        <v>332</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>942</v>
+        <v>263</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>943</v>
+        <v>266</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>944</v>
+        <v>334</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>946</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>947</v>
+        <v>935</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1083</v>
+        <v>936</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>955</v>
+        <v>942</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>954</v>
+        <v>943</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1117</v>
+        <v>1082</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>1001</v>
+        <v>946</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>962</v>
+        <v>947</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1085</v>
+        <v>949</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>963</v>
+        <v>950</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1078</v>
+        <v>951</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>265</v>
+        <v>952</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>964</v>
+        <v>953</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>263</v>
+        <v>955</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>266</v>
+        <v>954</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>967</v>
+        <v>956</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1086</v>
+        <v>1117</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>969</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>970</v>
+        <v>962</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>971</v>
+        <v>1084</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>972</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>975</v>
+        <v>963</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1087</v>
+        <v>1078</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1088</v>
+        <v>265</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>978</v>
+        <v>964</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>979</v>
+        <v>263</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>980</v>
+        <v>266</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>983</v>
+        <v>967</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>984</v>
+        <v>1086</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>985</v>
+        <v>969</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>1006</v>
+        <v>970</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1090</v>
+        <v>971</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>1007</v>
+        <v>972</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1008</v>
+        <v>975</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1009</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>1010</v>
+        <v>978</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>1011</v>
+        <v>979</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1012</v>
+        <v>980</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>1013</v>
+        <v>983</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>1014</v>
+        <v>984</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>1015</v>
+        <v>985</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1016</v>
+        <v>1006</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1017</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>1130</v>
+        <v>1008</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>1132</v>
+        <v>1091</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1131</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>1135</v>
+        <v>1010</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>1137</v>
+        <v>1011</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>1136</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>1138</v>
+        <v>1013</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>1139</v>
+        <v>1014</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>1140</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>1141</v>
+        <v>1016</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1143</v>
+        <v>1092</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1142</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>1144</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B150" s="1" t="s">
         <v>1145</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C150" s="1" t="s">
         <v>1146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.2.2 add welcome text
</commit_message>
<xml_diff>
--- a/src/locales/translations.xlsx
+++ b/src/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\icmm-web\src\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D99F5DC-12FE-4384-935D-99BEBFB4B6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17863427-EC43-4004-BE1B-A824A88B23D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B932D239-48A5-4026-8CCD-CA2BFDECA8AC}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="1192">
   <si>
     <t>id</t>
   </si>
@@ -3616,6 +3616,34 @@
   </si>
   <si>
     <t>ผ้าบัฟ รุ่น Coolnet UV + กางเกงวิ่งขาสั้นหญิง 3 นิ้ว</t>
+  </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <t>Notice…</t>
+  </si>
+  <si>
+    <t>ประกาศ…</t>
+  </si>
+  <si>
+    <t>preorderTxt</t>
+  </si>
+  <si>
+    <t>This product is Pre-Order.
+Estimated shipping: New Year 2026.</t>
+  </si>
+  <si>
+    <t>สินค้าเป็นแบบ Pre-Order จัดส่งสินค้าช่วงปีใหม่ 2026</t>
+  </si>
+  <si>
+    <t>accept</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>ยอมรับ</t>
   </si>
 </sst>
 </file>
@@ -4000,10 +4028,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EFFCAA-6DA9-40A3-BF28-CA3BC524DD9C}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5660,6 +5688,39 @@
       </c>
       <c r="C150" s="1" t="s">
         <v>1146</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>1191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>